<commit_message>
New rules and template for K32-Kurzaktivität
</commit_message>
<xml_diff>
--- a/dragonlog/contest/data/Logvorlage_V1_FM_K32.xlsx
+++ b/dragonlog/contest/data/Logvorlage_V1_FM_K32.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Funk\DragonLog\dragonlog\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Funk\DragonLog\dragonlog\contest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84DB54D-06FF-4DDE-B512-A98F299B73E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7222A119-317C-47D9-8380-DF59384F0D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29835" yWindow="720" windowWidth="22260" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Log!$7:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Log!$8:$9</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,18 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Mittelrhein-FM-Kurzaktivität</t>
   </si>
   <si>
     <t>Uhrzeit UTC</t>
-  </si>
-  <si>
-    <t>Anschrift:</t>
-  </si>
-  <si>
-    <t>DOK:</t>
   </si>
   <si>
     <t>Kategorie:</t>
@@ -48,37 +42,37 @@
     <t>E-Mail:</t>
   </si>
   <si>
-    <t>Kategorie Gegenstation</t>
-  </si>
-  <si>
-    <t>Eigenes Call:</t>
-  </si>
-  <si>
-    <t>PLZ Wohnort:</t>
-  </si>
-  <si>
     <t>Name, Vorname:</t>
   </si>
   <si>
     <t>Datum:</t>
   </si>
   <si>
-    <t>2m / 70cm</t>
-  </si>
-  <si>
     <t>A  // B  //  C</t>
-  </si>
-  <si>
-    <t>Band:</t>
   </si>
   <si>
     <t>Gearbeitete Station</t>
   </si>
   <si>
-    <t>DOK  Gegenstation</t>
+    <t>Locator 
+Standort:</t>
   </si>
   <si>
-    <t>Locator Standort:</t>
+    <t>Eigenes Rufzeichen:</t>
+  </si>
+  <si>
+    <t>Eigener DOK:</t>
+  </si>
+  <si>
+    <t>Kategorie 
+Gegenstation</t>
+  </si>
+  <si>
+    <t>DOK  
+Gegenstation</t>
+  </si>
+  <si>
+    <t>Band (2/70)</t>
   </si>
 </sst>
 </file>
@@ -88,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +128,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -149,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -188,13 +197,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -210,66 +219,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -306,6 +255,43 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -313,29 +299,77 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,56 +379,81 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,361 +769,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="1"/>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1"/>
-      <c r="C2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:6" s="21" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20">
+        <v>2</v>
+      </c>
+      <c r="C8" s="19">
+        <v>3</v>
+      </c>
+      <c r="D8" s="19">
+        <v>4</v>
+      </c>
+      <c r="E8" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>